<commit_message>
Fix a bug with non integer group counts
</commit_message>
<xml_diff>
--- a/data/L2-MS.xlsx
+++ b/data/L2-MS.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/SSDS/enseignement/UFR STAPS/Direction/Outils/celcatreport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C20A5C-4581-3C48-AD8E-35E4AF9B73B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA7E08C-0884-F44C-B468-4423900CB1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19580" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19560" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
   </bookViews>
   <sheets>
     <sheet name="L2-MS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D425352-B3D2-6642-82B3-EC9BD51219AA}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>